<commit_message>
Remove duplication in df4
Due to each data point being registered in two projects
</commit_message>
<xml_diff>
--- a/Data/05_TBT.xlsx
+++ b/Data/05_TBT.xlsx
@@ -2216,293 +2216,319 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B68" t="n">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="C68" t="s">
-        <v>49</v>
-      </c>
-      <c r="D68"/>
+        <v>30</v>
+      </c>
+      <c r="D68" t="s">
+        <v>60</v>
+      </c>
       <c r="E68" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F68" t="n">
-        <v>16.6</v>
+        <v>590</v>
       </c>
       <c r="G68"/>
       <c r="H68" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B69" t="n">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="C69" t="s">
-        <v>49</v>
-      </c>
-      <c r="D69"/>
+        <v>30</v>
+      </c>
+      <c r="D69" t="s">
+        <v>63</v>
+      </c>
       <c r="E69" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="F69" t="n">
-        <v>8.3</v>
+        <v>1200</v>
       </c>
       <c r="G69"/>
       <c r="H69" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B70" t="n">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="C70" t="s">
-        <v>49</v>
-      </c>
-      <c r="D70"/>
+        <v>30</v>
+      </c>
+      <c r="D70" t="s">
+        <v>65</v>
+      </c>
       <c r="E70" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="F70" t="n">
-        <v>12</v>
+        <v>1400</v>
       </c>
       <c r="G70"/>
       <c r="H70" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B71" t="n">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="C71" t="s">
-        <v>49</v>
-      </c>
-      <c r="D71"/>
+        <v>30</v>
+      </c>
+      <c r="D71" t="s">
+        <v>66</v>
+      </c>
       <c r="E71" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F71" t="n">
-        <v>20</v>
+        <v>1500</v>
       </c>
       <c r="G71"/>
       <c r="H71" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B72" t="n">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="C72" t="s">
-        <v>49</v>
-      </c>
-      <c r="D72"/>
+        <v>30</v>
+      </c>
+      <c r="D72" t="s">
+        <v>67</v>
+      </c>
       <c r="E72" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F72" t="n">
-        <v>43</v>
+        <v>1500</v>
       </c>
       <c r="G72"/>
       <c r="H72" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="B73" t="n">
-        <v>2016</v>
+        <v>2005</v>
       </c>
       <c r="C73" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73"/>
+        <v>30</v>
+      </c>
+      <c r="D73" t="s">
+        <v>68</v>
+      </c>
       <c r="E73" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F73" t="n">
-        <v>1</v>
+        <v>1500</v>
       </c>
       <c r="G73"/>
       <c r="H73" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="B74" t="n">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
-      </c>
-      <c r="D74"/>
+        <v>30</v>
+      </c>
+      <c r="D74" t="s">
+        <v>69</v>
+      </c>
       <c r="E74" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F74" t="n">
-        <v>1.4</v>
+        <v>1100</v>
       </c>
       <c r="G74"/>
       <c r="H74" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B75" t="n">
-        <v>2016</v>
+        <v>2005</v>
       </c>
       <c r="C75" t="s">
-        <v>9</v>
-      </c>
-      <c r="D75"/>
+        <v>30</v>
+      </c>
+      <c r="D75" t="s">
+        <v>70</v>
+      </c>
       <c r="E75" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F75" t="n">
-        <v>11.6</v>
+        <v>1000</v>
       </c>
       <c r="G75"/>
       <c r="H75" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B76" t="n">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="C76" t="s">
-        <v>9</v>
-      </c>
-      <c r="D76"/>
+        <v>30</v>
+      </c>
+      <c r="D76" t="s">
+        <v>71</v>
+      </c>
       <c r="E76" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F76" t="n">
-        <v>6.4</v>
+        <v>590</v>
       </c>
       <c r="G76"/>
       <c r="H76" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B77" t="n">
-        <v>2016</v>
+        <v>2005</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
-      </c>
-      <c r="D77"/>
+        <v>30</v>
+      </c>
+      <c r="D77" t="s">
+        <v>72</v>
+      </c>
       <c r="E77" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F77" t="n">
-        <v>104</v>
+        <v>380</v>
       </c>
       <c r="G77"/>
       <c r="H77" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B78" t="n">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="C78" t="s">
-        <v>9</v>
-      </c>
-      <c r="D78"/>
+        <v>30</v>
+      </c>
+      <c r="D78" t="s">
+        <v>73</v>
+      </c>
       <c r="E78" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F78" t="n">
-        <v>64</v>
+        <v>160</v>
       </c>
       <c r="G78"/>
       <c r="H78" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B79" t="n">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="C79" t="s">
-        <v>9</v>
-      </c>
-      <c r="D79"/>
+        <v>30</v>
+      </c>
+      <c r="D79" t="s">
+        <v>60</v>
+      </c>
       <c r="E79" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F79" t="n">
-        <v>51.4</v>
+        <v>760</v>
       </c>
       <c r="G79"/>
       <c r="H79" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B80" t="n">
-        <v>2018</v>
+        <v>2004</v>
       </c>
       <c r="C80" t="s">
-        <v>9</v>
-      </c>
-      <c r="D80"/>
+        <v>30</v>
+      </c>
+      <c r="D80" t="s">
+        <v>60</v>
+      </c>
       <c r="E80" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F80" t="n">
-        <v>29</v>
+        <v>950</v>
       </c>
       <c r="G80"/>
       <c r="H80" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="B81" t="n">
         <v>2004</v>
@@ -2514,10 +2540,10 @@
         <v>60</v>
       </c>
       <c r="E81" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="F81" t="n">
-        <v>590</v>
+        <v>16000</v>
       </c>
       <c r="G81"/>
       <c r="H81" t="s">
@@ -2526,22 +2552,22 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="B82" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C82" t="s">
         <v>30</v>
       </c>
       <c r="D82" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E82" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="F82" t="n">
-        <v>1200</v>
+        <v>54000</v>
       </c>
       <c r="G82"/>
       <c r="H82" t="s">
@@ -2550,22 +2576,22 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="B83" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C83" t="s">
         <v>30</v>
       </c>
       <c r="D83" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E83" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="F83" t="n">
-        <v>1400</v>
+        <v>63000</v>
       </c>
       <c r="G83"/>
       <c r="H83" t="s">
@@ -2574,22 +2600,22 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B84" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C84" t="s">
         <v>30</v>
       </c>
       <c r="D84" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E84" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="F84" t="n">
-        <v>1500</v>
+        <v>18000</v>
       </c>
       <c r="G84"/>
       <c r="H84" t="s">
@@ -2598,22 +2624,22 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C85" t="s">
         <v>30</v>
       </c>
       <c r="D85" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E85" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="F85" t="n">
-        <v>1500</v>
+        <v>16000</v>
       </c>
       <c r="G85"/>
       <c r="H85" t="s">
@@ -2622,22 +2648,22 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C86" t="s">
         <v>30</v>
       </c>
       <c r="D86" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E86" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="F86" t="n">
-        <v>1500</v>
+        <v>3600</v>
       </c>
       <c r="G86"/>
       <c r="H86" t="s">
@@ -2646,22 +2672,22 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C87" t="s">
         <v>30</v>
       </c>
       <c r="D87" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E87" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="F87" t="n">
-        <v>1100</v>
+        <v>7800</v>
       </c>
       <c r="G87"/>
       <c r="H87" t="s">
@@ -2670,22 +2696,22 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B88" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C88" t="s">
         <v>30</v>
       </c>
       <c r="D88" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E88" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="F88" t="n">
-        <v>1000</v>
+        <v>6400</v>
       </c>
       <c r="G88"/>
       <c r="H88" t="s">
@@ -2694,22 +2720,22 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B89" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C89" t="s">
         <v>30</v>
       </c>
       <c r="D89" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E89" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="F89" t="n">
-        <v>590</v>
+        <v>7000</v>
       </c>
       <c r="G89"/>
       <c r="H89" t="s">
@@ -2718,22 +2744,22 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B90" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C90" t="s">
         <v>30</v>
       </c>
       <c r="D90" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E90" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="F90" t="n">
-        <v>380</v>
+        <v>6200</v>
       </c>
       <c r="G90"/>
       <c r="H90" t="s">
@@ -2742,22 +2768,22 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B91" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C91" t="s">
         <v>30</v>
       </c>
       <c r="D91" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E91" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="F91" t="n">
-        <v>160</v>
+        <v>8900</v>
       </c>
       <c r="G91"/>
       <c r="H91" t="s">
@@ -2766,7 +2792,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="B92" t="n">
         <v>2004</v>
@@ -2775,13 +2801,13 @@
         <v>30</v>
       </c>
       <c r="D92" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E92" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="F92" t="n">
-        <v>760</v>
+        <v>5700</v>
       </c>
       <c r="G92"/>
       <c r="H92" t="s">
@@ -2790,7 +2816,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="B93" t="n">
         <v>2004</v>
@@ -2799,13 +2825,13 @@
         <v>30</v>
       </c>
       <c r="D93" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E93" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="F93" t="n">
-        <v>950</v>
+        <v>2800</v>
       </c>
       <c r="G93"/>
       <c r="H93" t="s">
@@ -2814,7 +2840,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="B94" t="n">
         <v>2004</v>
@@ -2823,13 +2849,13 @@
         <v>30</v>
       </c>
       <c r="D94" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="E94" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F94" t="n">
-        <v>16000</v>
+        <v>1400</v>
       </c>
       <c r="G94"/>
       <c r="H94" t="s">
@@ -2838,7 +2864,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B95" t="n">
         <v>2004</v>
@@ -2847,13 +2873,13 @@
         <v>30</v>
       </c>
       <c r="D95" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="E95" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="F95" t="n">
-        <v>54000</v>
+        <v>720</v>
       </c>
       <c r="G95"/>
       <c r="H95" t="s">
@@ -2862,7 +2888,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B96" t="n">
         <v>2004</v>
@@ -2871,13 +2897,13 @@
         <v>30</v>
       </c>
       <c r="D96" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E96" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F96" t="n">
-        <v>63000</v>
+        <v>540</v>
       </c>
       <c r="G96"/>
       <c r="H96" t="s">
@@ -2886,7 +2912,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B97" t="n">
         <v>2004</v>
@@ -2898,10 +2924,10 @@
         <v>60</v>
       </c>
       <c r="E97" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F97" t="n">
-        <v>18000</v>
+        <v>3600</v>
       </c>
       <c r="G97"/>
       <c r="H97" t="s">
@@ -2910,22 +2936,22 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B98" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C98" t="s">
         <v>30</v>
       </c>
       <c r="D98" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E98" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F98" t="n">
-        <v>16000</v>
+        <v>3800</v>
       </c>
       <c r="G98"/>
       <c r="H98" t="s">
@@ -2934,22 +2960,22 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B99" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C99" t="s">
         <v>30</v>
       </c>
       <c r="D99" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E99" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F99" t="n">
-        <v>3600</v>
+        <v>3900</v>
       </c>
       <c r="G99"/>
       <c r="H99" t="s">
@@ -2958,22 +2984,22 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B100" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C100" t="s">
         <v>30</v>
       </c>
       <c r="D100" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E100" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F100" t="n">
-        <v>7800</v>
+        <v>4300</v>
       </c>
       <c r="G100"/>
       <c r="H100" t="s">
@@ -2982,22 +3008,22 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B101" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C101" t="s">
         <v>30</v>
       </c>
       <c r="D101" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E101" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F101" t="n">
-        <v>6400</v>
+        <v>3600</v>
       </c>
       <c r="G101"/>
       <c r="H101" t="s">
@@ -3006,22 +3032,22 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B102" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C102" t="s">
         <v>30</v>
       </c>
       <c r="D102" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E102" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F102" t="n">
-        <v>7000</v>
+        <v>3600</v>
       </c>
       <c r="G102"/>
       <c r="H102" t="s">
@@ -3030,22 +3056,22 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B103" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C103" t="s">
         <v>30</v>
       </c>
       <c r="D103" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E103" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F103" t="n">
-        <v>6200</v>
+        <v>2500</v>
       </c>
       <c r="G103"/>
       <c r="H103" t="s">
@@ -3054,22 +3080,22 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B104" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C104" t="s">
         <v>30</v>
       </c>
       <c r="D104" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E104" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F104" t="n">
-        <v>8900</v>
+        <v>910</v>
       </c>
       <c r="G104"/>
       <c r="H104" t="s">
@@ -3078,22 +3104,22 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B105" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C105" t="s">
         <v>30</v>
       </c>
       <c r="D105" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E105" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F105" t="n">
-        <v>5700</v>
+        <v>330</v>
       </c>
       <c r="G105"/>
       <c r="H105" t="s">
@@ -3102,22 +3128,22 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B106" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C106" t="s">
         <v>30</v>
       </c>
       <c r="D106" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E106" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F106" t="n">
-        <v>2800</v>
+        <v>200</v>
       </c>
       <c r="G106"/>
       <c r="H106" t="s">
@@ -3126,22 +3152,22 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B107" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C107" t="s">
         <v>30</v>
       </c>
       <c r="D107" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E107" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F107" t="n">
-        <v>1400</v>
+        <v>200</v>
       </c>
       <c r="G107"/>
       <c r="H107" t="s">
@@ -3150,7 +3176,7 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B108" t="n">
         <v>2004</v>
@@ -3159,13 +3185,13 @@
         <v>30</v>
       </c>
       <c r="D108" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E108" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F108" t="n">
-        <v>720</v>
+        <v>7500</v>
       </c>
       <c r="G108"/>
       <c r="H108" t="s">
@@ -3174,7 +3200,7 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B109" t="n">
         <v>2004</v>
@@ -3183,13 +3209,13 @@
         <v>30</v>
       </c>
       <c r="D109" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="E109" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F109" t="n">
-        <v>540</v>
+        <v>800</v>
       </c>
       <c r="G109"/>
       <c r="H109" t="s">
@@ -3198,7 +3224,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B110" t="n">
         <v>2004</v>
@@ -3210,10 +3236,10 @@
         <v>60</v>
       </c>
       <c r="E110" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F110" t="n">
-        <v>3600</v>
+        <v>5100</v>
       </c>
       <c r="G110"/>
       <c r="H110" t="s">
@@ -3222,22 +3248,22 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B111" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C111" t="s">
         <v>30</v>
       </c>
       <c r="D111" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E111" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F111" t="n">
-        <v>3800</v>
+        <v>17000</v>
       </c>
       <c r="G111"/>
       <c r="H111" t="s">
@@ -3246,489 +3272,489 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="B112" t="n">
         <v>2005</v>
       </c>
       <c r="C112" t="s">
-        <v>30</v>
-      </c>
-      <c r="D112" t="s">
-        <v>65</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D112"/>
       <c r="E112" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="F112" t="n">
-        <v>3900</v>
+        <v>20</v>
       </c>
       <c r="G112"/>
       <c r="H112" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="B113" t="n">
         <v>2005</v>
       </c>
       <c r="C113" t="s">
-        <v>30</v>
-      </c>
-      <c r="D113" t="s">
-        <v>66</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D113"/>
       <c r="E113" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="F113" t="n">
-        <v>4300</v>
+        <v>29</v>
       </c>
       <c r="G113"/>
       <c r="H113" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="B114" t="n">
         <v>2005</v>
       </c>
       <c r="C114" t="s">
-        <v>30</v>
-      </c>
-      <c r="D114" t="s">
-        <v>67</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D114"/>
       <c r="E114" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="F114" t="n">
-        <v>3600</v>
+        <v>180</v>
       </c>
       <c r="G114"/>
       <c r="H114" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="B115" t="n">
         <v>2005</v>
       </c>
       <c r="C115" t="s">
-        <v>30</v>
-      </c>
-      <c r="D115" t="s">
-        <v>68</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D115"/>
       <c r="E115" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="F115" t="n">
-        <v>3600</v>
+        <v>150</v>
       </c>
       <c r="G115"/>
       <c r="H115" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="B116" t="n">
         <v>2005</v>
       </c>
       <c r="C116" t="s">
-        <v>30</v>
-      </c>
-      <c r="D116" t="s">
-        <v>69</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D116"/>
       <c r="E116" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="F116" t="n">
-        <v>2500</v>
+        <v>130</v>
       </c>
       <c r="G116"/>
       <c r="H116" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>87</v>
+        <v>8</v>
       </c>
       <c r="B117" t="n">
         <v>2005</v>
       </c>
       <c r="C117" t="s">
-        <v>30</v>
-      </c>
-      <c r="D117" t="s">
-        <v>70</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D117"/>
       <c r="E117" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="F117" t="n">
-        <v>910</v>
+        <v>850</v>
       </c>
       <c r="G117"/>
       <c r="H117" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="B118" t="n">
         <v>2005</v>
       </c>
       <c r="C118" t="s">
-        <v>30</v>
-      </c>
-      <c r="D118" t="s">
-        <v>71</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D118"/>
       <c r="E118" t="s">
-        <v>88</v>
-      </c>
-      <c r="F118" t="n">
-        <v>330</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="F118"/>
       <c r="G118"/>
       <c r="H118" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="s">
-        <v>87</v>
-      </c>
+      <c r="A119"/>
       <c r="B119" t="n">
         <v>2005</v>
       </c>
       <c r="C119" t="s">
-        <v>30</v>
-      </c>
-      <c r="D119" t="s">
-        <v>72</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D119"/>
       <c r="E119" t="s">
-        <v>88</v>
-      </c>
-      <c r="F119" t="n">
-        <v>200</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F119"/>
       <c r="G119"/>
       <c r="H119" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="B120" t="n">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="C120" t="s">
         <v>30</v>
       </c>
       <c r="D120" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="E120" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="F120" t="n">
-        <v>200</v>
+        <v>1600</v>
       </c>
       <c r="G120"/>
       <c r="H120" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="B121" t="n">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="C121" t="s">
         <v>30</v>
       </c>
       <c r="D121" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="E121" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="F121" t="n">
-        <v>7500</v>
+        <v>320</v>
       </c>
       <c r="G121"/>
       <c r="H121" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="B122" t="n">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="C122" t="s">
         <v>30</v>
       </c>
       <c r="D122" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="E122" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="F122" t="n">
-        <v>800</v>
+        <v>960</v>
       </c>
       <c r="G122"/>
       <c r="H122" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
       <c r="B123" t="n">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="C123" t="s">
         <v>30</v>
       </c>
       <c r="D123" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="E123" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="F123" t="n">
-        <v>5100</v>
+        <v>93000</v>
       </c>
       <c r="G123"/>
       <c r="H123" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B124" t="n">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="C124" t="s">
         <v>30</v>
       </c>
       <c r="D124" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="E124" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="F124" t="n">
-        <v>17000</v>
+        <v>1500</v>
       </c>
       <c r="G124"/>
       <c r="H124" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="B125" t="n">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="C125" t="s">
-        <v>49</v>
-      </c>
-      <c r="D125"/>
+        <v>30</v>
+      </c>
+      <c r="D125" t="s">
+        <v>106</v>
+      </c>
       <c r="E125" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="F125" t="n">
-        <v>20</v>
+        <v>6200</v>
       </c>
       <c r="G125"/>
       <c r="H125" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="B126" t="n">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="C126" t="s">
-        <v>49</v>
-      </c>
-      <c r="D126"/>
+        <v>30</v>
+      </c>
+      <c r="D126" t="s">
+        <v>106</v>
+      </c>
       <c r="E126" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="F126" t="n">
-        <v>29</v>
+        <v>3700</v>
       </c>
       <c r="G126"/>
       <c r="H126" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>48</v>
+        <v>117</v>
       </c>
       <c r="B127" t="n">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="C127" t="s">
-        <v>49</v>
-      </c>
-      <c r="D127"/>
+        <v>30</v>
+      </c>
+      <c r="D127" t="s">
+        <v>106</v>
+      </c>
       <c r="E127" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="F127" t="n">
-        <v>180</v>
+        <v>4400</v>
       </c>
       <c r="G127"/>
       <c r="H127" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="B128" t="n">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="C128" t="s">
-        <v>49</v>
-      </c>
-      <c r="D128"/>
+        <v>30</v>
+      </c>
+      <c r="D128" t="s">
+        <v>106</v>
+      </c>
       <c r="E128" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="F128" t="n">
-        <v>150</v>
+        <v>2500</v>
       </c>
       <c r="G128"/>
       <c r="H128" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="B129" t="n">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="C129" t="s">
-        <v>49</v>
-      </c>
-      <c r="D129"/>
+        <v>30</v>
+      </c>
+      <c r="D129" t="s">
+        <v>106</v>
+      </c>
       <c r="E129" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="F129" t="n">
-        <v>130</v>
+        <v>1900</v>
       </c>
       <c r="G129"/>
       <c r="H129" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>8</v>
+        <v>123</v>
       </c>
       <c r="B130" t="n">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="C130" t="s">
-        <v>49</v>
-      </c>
-      <c r="D130"/>
+        <v>30</v>
+      </c>
+      <c r="D130" t="s">
+        <v>106</v>
+      </c>
       <c r="E130" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="F130" t="n">
-        <v>850</v>
+        <v>1800</v>
       </c>
       <c r="G130"/>
       <c r="H130" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="B131" t="n">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="C131" t="s">
-        <v>49</v>
-      </c>
-      <c r="D131"/>
+        <v>30</v>
+      </c>
+      <c r="D131" t="s">
+        <v>106</v>
+      </c>
       <c r="E131" t="s">
-        <v>104</v>
-      </c>
-      <c r="F131"/>
+        <v>126</v>
+      </c>
+      <c r="F131" t="n">
+        <v>860</v>
+      </c>
       <c r="G131"/>
       <c r="H131" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132"/>
+      <c r="A132" t="s">
+        <v>127</v>
+      </c>
       <c r="B132" t="n">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="C132" t="s">
-        <v>49</v>
-      </c>
-      <c r="D132"/>
+        <v>30</v>
+      </c>
+      <c r="D132" t="s">
+        <v>106</v>
+      </c>
       <c r="E132" t="s">
-        <v>105</v>
-      </c>
-      <c r="F132"/>
+        <v>128</v>
+      </c>
+      <c r="F132" t="n">
+        <v>1500</v>
+      </c>
       <c r="G132"/>
       <c r="H132" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>14</v>
+        <v>129</v>
       </c>
       <c r="B133" t="n">
         <v>2008</v>
@@ -3740,10 +3766,10 @@
         <v>106</v>
       </c>
       <c r="E133" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="F133" t="n">
-        <v>1600</v>
+        <v>770</v>
       </c>
       <c r="G133"/>
       <c r="H133" t="s">
@@ -3752,7 +3778,7 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="B134" t="n">
         <v>2008</v>
@@ -3764,10 +3790,10 @@
         <v>106</v>
       </c>
       <c r="E134" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="F134" t="n">
-        <v>320</v>
+        <v>1100</v>
       </c>
       <c r="G134"/>
       <c r="H134" t="s">
@@ -3776,7 +3802,7 @@
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="B135" t="n">
         <v>2008</v>
@@ -3788,10 +3814,10 @@
         <v>106</v>
       </c>
       <c r="E135" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="F135" t="n">
-        <v>960</v>
+        <v>1600</v>
       </c>
       <c r="G135"/>
       <c r="H135" t="s">
@@ -3800,314 +3826,288 @@
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B136" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C136" t="s">
-        <v>30</v>
-      </c>
-      <c r="D136" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D136"/>
       <c r="E136" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="F136" t="n">
-        <v>93000</v>
+        <v>55</v>
       </c>
       <c r="G136"/>
       <c r="H136" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="B137" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C137" t="s">
-        <v>30</v>
-      </c>
-      <c r="D137" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D137"/>
       <c r="E137" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="F137" t="n">
-        <v>1500</v>
+        <v>52</v>
       </c>
       <c r="G137"/>
       <c r="H137" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>113</v>
+        <v>15</v>
       </c>
       <c r="B138" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C138" t="s">
-        <v>30</v>
-      </c>
-      <c r="D138" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D138"/>
       <c r="E138" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="F138" t="n">
-        <v>6200</v>
+        <v>70</v>
       </c>
       <c r="G138"/>
       <c r="H138" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>115</v>
+        <v>15</v>
       </c>
       <c r="B139" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C139" t="s">
-        <v>30</v>
-      </c>
-      <c r="D139" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D139"/>
       <c r="E139" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="F139" t="n">
-        <v>3700</v>
+        <v>67</v>
       </c>
       <c r="G139"/>
       <c r="H139" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>117</v>
+        <v>8</v>
       </c>
       <c r="B140" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C140" t="s">
-        <v>30</v>
-      </c>
-      <c r="D140" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D140"/>
       <c r="E140" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="F140" t="n">
-        <v>4400</v>
+        <v>160</v>
       </c>
       <c r="G140"/>
       <c r="H140" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>119</v>
+        <v>8</v>
       </c>
       <c r="B141" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C141" t="s">
-        <v>30</v>
-      </c>
-      <c r="D141" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D141"/>
       <c r="E141" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="F141" t="n">
-        <v>2500</v>
+        <v>180</v>
       </c>
       <c r="G141"/>
       <c r="H141" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>121</v>
+        <v>16</v>
       </c>
       <c r="B142" t="n">
         <v>2008</v>
       </c>
       <c r="C142" t="s">
-        <v>30</v>
-      </c>
-      <c r="D142" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D142"/>
       <c r="E142" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="F142" t="n">
-        <v>1900</v>
+        <v>97</v>
       </c>
       <c r="G142"/>
       <c r="H142" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>123</v>
+        <v>16</v>
       </c>
       <c r="B143" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C143" t="s">
-        <v>30</v>
-      </c>
-      <c r="D143" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D143"/>
       <c r="E143" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="F143" t="n">
-        <v>1800</v>
+        <v>55</v>
       </c>
       <c r="G143"/>
       <c r="H143" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>125</v>
+        <v>16</v>
       </c>
       <c r="B144" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C144" t="s">
-        <v>30</v>
-      </c>
-      <c r="D144" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D144"/>
       <c r="E144" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="F144" t="n">
-        <v>860</v>
+        <v>52</v>
       </c>
       <c r="G144"/>
       <c r="H144" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>127</v>
+        <v>15</v>
       </c>
       <c r="B145" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C145" t="s">
-        <v>30</v>
-      </c>
-      <c r="D145" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D145"/>
       <c r="E145" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="F145" t="n">
-        <v>1500</v>
+        <v>70</v>
       </c>
       <c r="G145"/>
       <c r="H145" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>129</v>
+        <v>15</v>
       </c>
       <c r="B146" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C146" t="s">
-        <v>30</v>
-      </c>
-      <c r="D146" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D146"/>
       <c r="E146" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="F146" t="n">
-        <v>770</v>
+        <v>67</v>
       </c>
       <c r="G146"/>
       <c r="H146" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="B147" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C147" t="s">
-        <v>30</v>
-      </c>
-      <c r="D147" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D147"/>
       <c r="E147" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="F147" t="n">
-        <v>1100</v>
+        <v>160</v>
       </c>
       <c r="G147"/>
       <c r="H147" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="B148" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C148" t="s">
-        <v>30</v>
-      </c>
-      <c r="D148" t="s">
-        <v>106</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D148"/>
       <c r="E148" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="F148" t="n">
-        <v>1600</v>
+        <v>180</v>
       </c>
       <c r="G148"/>
       <c r="H148" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
     </row>
     <row r="149">
@@ -4122,14 +4122,14 @@
       </c>
       <c r="D149"/>
       <c r="E149" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="F149" t="n">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="G149"/>
       <c r="H149" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="150">
@@ -4144,14 +4144,14 @@
       </c>
       <c r="D150"/>
       <c r="E150" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="F150" t="n">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="G150"/>
       <c r="H150" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="151">
@@ -4166,14 +4166,14 @@
       </c>
       <c r="D151"/>
       <c r="E151" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F151" t="n">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="G151"/>
       <c r="H151" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="152">
@@ -4188,14 +4188,14 @@
       </c>
       <c r="D152"/>
       <c r="E152" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="F152" t="n">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="G152"/>
       <c r="H152" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="153">
@@ -4210,14 +4210,14 @@
       </c>
       <c r="D153"/>
       <c r="E153" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="F153" t="n">
-        <v>160</v>
+        <v>540</v>
       </c>
       <c r="G153"/>
       <c r="H153" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="154">
@@ -4232,299 +4232,13 @@
       </c>
       <c r="D154"/>
       <c r="E154" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="F154" t="n">
-        <v>180</v>
+        <v>500</v>
       </c>
       <c r="G154"/>
       <c r="H154" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="s">
-        <v>16</v>
-      </c>
-      <c r="B155" t="n">
-        <v>2008</v>
-      </c>
-      <c r="C155" t="s">
-        <v>49</v>
-      </c>
-      <c r="D155"/>
-      <c r="E155" t="s">
-        <v>142</v>
-      </c>
-      <c r="F155" t="n">
-        <v>97</v>
-      </c>
-      <c r="G155"/>
-      <c r="H155" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="s">
-        <v>16</v>
-      </c>
-      <c r="B156" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C156" t="s">
-        <v>49</v>
-      </c>
-      <c r="D156"/>
-      <c r="E156" t="s">
-        <v>135</v>
-      </c>
-      <c r="F156" t="n">
-        <v>55</v>
-      </c>
-      <c r="G156"/>
-      <c r="H156" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="s">
-        <v>16</v>
-      </c>
-      <c r="B157" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C157" t="s">
-        <v>49</v>
-      </c>
-      <c r="D157"/>
-      <c r="E157" t="s">
-        <v>137</v>
-      </c>
-      <c r="F157" t="n">
-        <v>52</v>
-      </c>
-      <c r="G157"/>
-      <c r="H157" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="s">
-        <v>15</v>
-      </c>
-      <c r="B158" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C158" t="s">
-        <v>49</v>
-      </c>
-      <c r="D158"/>
-      <c r="E158" t="s">
-        <v>138</v>
-      </c>
-      <c r="F158" t="n">
-        <v>70</v>
-      </c>
-      <c r="G158"/>
-      <c r="H158" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="s">
-        <v>15</v>
-      </c>
-      <c r="B159" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C159" t="s">
-        <v>49</v>
-      </c>
-      <c r="D159"/>
-      <c r="E159" t="s">
-        <v>139</v>
-      </c>
-      <c r="F159" t="n">
-        <v>67</v>
-      </c>
-      <c r="G159"/>
-      <c r="H159" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="s">
-        <v>8</v>
-      </c>
-      <c r="B160" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C160" t="s">
-        <v>49</v>
-      </c>
-      <c r="D160"/>
-      <c r="E160" t="s">
-        <v>140</v>
-      </c>
-      <c r="F160" t="n">
-        <v>160</v>
-      </c>
-      <c r="G160"/>
-      <c r="H160" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="s">
-        <v>8</v>
-      </c>
-      <c r="B161" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C161" t="s">
-        <v>49</v>
-      </c>
-      <c r="D161"/>
-      <c r="E161" t="s">
-        <v>141</v>
-      </c>
-      <c r="F161" t="n">
-        <v>180</v>
-      </c>
-      <c r="G161"/>
-      <c r="H161" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="s">
-        <v>16</v>
-      </c>
-      <c r="B162" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C162" t="s">
-        <v>49</v>
-      </c>
-      <c r="D162"/>
-      <c r="E162" t="s">
-        <v>142</v>
-      </c>
-      <c r="F162" t="n">
-        <v>97</v>
-      </c>
-      <c r="G162"/>
-      <c r="H162" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="s">
-        <v>16</v>
-      </c>
-      <c r="B163" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C163" t="s">
-        <v>49</v>
-      </c>
-      <c r="D163"/>
-      <c r="E163" t="s">
-        <v>144</v>
-      </c>
-      <c r="F163" t="n">
-        <v>85</v>
-      </c>
-      <c r="G163"/>
-      <c r="H163" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="s">
-        <v>15</v>
-      </c>
-      <c r="B164" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C164" t="s">
-        <v>49</v>
-      </c>
-      <c r="D164"/>
-      <c r="E164" t="s">
-        <v>145</v>
-      </c>
-      <c r="F164" t="n">
-        <v>83</v>
-      </c>
-      <c r="G164"/>
-      <c r="H164" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="s">
-        <v>15</v>
-      </c>
-      <c r="B165" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C165" t="s">
-        <v>49</v>
-      </c>
-      <c r="D165"/>
-      <c r="E165" t="s">
-        <v>146</v>
-      </c>
-      <c r="F165" t="n">
-        <v>82</v>
-      </c>
-      <c r="G165"/>
-      <c r="H165" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="s">
-        <v>8</v>
-      </c>
-      <c r="B166" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C166" t="s">
-        <v>49</v>
-      </c>
-      <c r="D166"/>
-      <c r="E166" t="s">
-        <v>147</v>
-      </c>
-      <c r="F166" t="n">
-        <v>540</v>
-      </c>
-      <c r="G166"/>
-      <c r="H166" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="s">
-        <v>8</v>
-      </c>
-      <c r="B167" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C167" t="s">
-        <v>49</v>
-      </c>
-      <c r="D167"/>
-      <c r="E167" t="s">
-        <v>148</v>
-      </c>
-      <c r="F167" t="n">
-        <v>500</v>
-      </c>
-      <c r="G167"/>
-      <c r="H167" t="s">
         <v>143</v>
       </c>
     </row>

</xml_diff>